<commit_message>
login asscociated files modify
</commit_message>
<xml_diff>
--- a/table_list.xlsx
+++ b/table_list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Database-Final-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\DB_final\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Annoucement</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,13 +72,29 @@
   </si>
   <si>
     <t>description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Account</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -426,15 +442,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,24 +463,36 @@
       <c r="E1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -472,17 +500,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
         <v>12</v>
       </c>
@@ -490,6 +518,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
login asscociated files modify 1
</commit_message>
<xml_diff>
--- a/table_list.xlsx
+++ b/table_list.xlsx
@@ -83,11 +83,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Password</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Account</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_pass</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -445,10 +445,13 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -467,7 +470,7 @@
         <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -489,7 +492,7 @@
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
login & logout & 初步區分admin(上方欄位&announce)
</commit_message>
<xml_diff>
--- a/table_list.xlsx
+++ b/table_list.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Annoucement</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -88,6 +88,10 @@
   </si>
   <si>
     <t>user_pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>authority</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -445,7 +449,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -501,6 +505,9 @@
       </c>
       <c r="E4" t="s">
         <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add column 'name' in user table
</commit_message>
<xml_diff>
--- a/table_list.xlsx
+++ b/table_list.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\DB_final\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="48" windowWidth="10752" windowHeight="7620"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="10755" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Annoucement</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -115,14 +110,22 @@
   </si>
   <si>
     <t>備註:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -234,7 +237,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -266,10 +269,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -301,7 +303,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -477,20 +478,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1"/>
-    <col min="10" max="10" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="10" max="10" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,7 +514,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -521,13 +522,13 @@
         <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -535,13 +536,13 @@
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -549,34 +550,40 @@
         <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="E5" t="s">
         <v>10</v>
       </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
       <c r="J5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="E6" t="s">
         <v>11</v>
       </c>
       <c r="J6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10">
       <c r="E7" t="s">
         <v>12</v>
+      </c>
+      <c r="J7" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -587,12 +594,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -600,12 +607,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix bugs of status.php
</commit_message>
<xml_diff>
--- a/table_list.xlsx
+++ b/table_list.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\DB_final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Homework\2017 Spring\Database System\Final\Final_Project\Database-Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="48" windowWidth="10752" windowHeight="7620"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="10755" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>Annoucement</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -139,10 +139,6 @@
   </si>
   <si>
     <t>varchar(50)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>datetime</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -294,8 +290,36 @@
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -597,22 +621,22 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,7 +644,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
@@ -638,21 +662,21 @@
         <v>15</v>
       </c>
       <c r="K1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" t="s">
         <v>48</v>
       </c>
-      <c r="L1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -661,7 +685,7 @@
         <v>29</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J2" t="s">
         <v>25</v>
@@ -670,21 +694,21 @@
         <v>24</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="J3" t="s">
         <v>14</v>
@@ -693,21 +717,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J4" t="s">
         <v>16</v>
@@ -719,12 +743,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J5" t="s">
         <v>17</v>
@@ -736,94 +760,94 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
         <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
         <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
         <v>39</v>
-      </c>
-      <c r="B11" t="s">
-        <v>40</v>
       </c>
       <c r="C11" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" t="s">
         <v>42</v>
       </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>43</v>
       </c>
-      <c r="G12" t="s">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>45</v>
       </c>
       <c r="C13" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G13" t="s">
         <v>28</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -839,7 +863,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -852,7 +876,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>